<commit_message>
Update Deploy and Execute Function
</commit_message>
<xml_diff>
--- a/Configuration/test_data.xlsx
+++ b/Configuration/test_data.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8976" windowWidth="23316" xWindow="30060" yWindow="4392"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="17616" windowWidth="29016" xWindow="28692" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="UUT" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Config" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PreparedTemplates" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="createTemplate" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Config" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="UUT_HP ThinPro 7" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="UUT_WES7P-64" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="UUT_Win10IoT-64" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="UUT_WES7E" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="PreparedTemplates" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="createTemplate" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -389,42 +392,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet5">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
-    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
-    <col customWidth="1" max="256" min="3" style="1" width="9.109375"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="11.88671875"/>
+    <col customWidth="1" max="2" min="2" style="1" width="43.88671875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="21.88671875"/>
+    <col customWidth="1" max="257" min="4" style="1" width="9.109375"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>Project Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Mac</t>
+          <t>Local Path</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>OS</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2"/>
-    <row customFormat="1" r="3" s="2"/>
+          <t>Remote Path</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Windows_precheck</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>c:\inetpub\ftproot\C:\inetpub\ftproot\jenkins\windows\task_2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>c:\temp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
@@ -441,35 +460,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet2">
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.44140625"/>
-    <col customWidth="1" max="2" min="2" style="1" width="11.5546875"/>
-    <col customWidth="1" max="256" min="3" style="1" width="9.109375"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="4" min="3" style="1" width="9.109375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="20.5546875"/>
+    <col customWidth="1" max="256" min="6" style="1" width="9.109375"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Local Path</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Remote Path</t>
-        </is>
-      </c>
-    </row>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
@@ -486,130 +523,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet3">
+  <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1:D65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="2" min="1" style="1" width="27.88671875"/>
-    <col customWidth="1" max="3" min="3" style="1" width="22.44140625"/>
-    <col customWidth="1" max="4" min="4" style="1" width="27.21875"/>
-    <col customWidth="1" max="5" min="5" style="1" width="22.44140625"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="4" min="3" style="1" width="9.109375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="14"/>
     <col customWidth="1" max="256" min="6" style="1" width="9.109375"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.75" r="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>WES10IoT-64</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>WES7E</t>
+          <t>Mac</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>WES7P-64</t>
+          <t>capture id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>HP ThinPro 7</t>
+          <t>deploy id</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>HP ThinPro 6-64</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>CaptureFiles_WES10IoT-64</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>CaptureFiles_WES7E</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>CaptureFiles_WES7P-64</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>CaptureFiles_HP ThinPro 7</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>CaptureFiles_HP ThinPro 6-64</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" r="3" s="2">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Command_WES10IoT-64</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Command_WES7E</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Command_WES7P-64</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Command_HP ThinPro 7</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Command_HP ThinPro 6-64</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" r="4" s="2">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Files_WES10IoT-64</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Files_WES7E</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Files_WES7P-64</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Files_HP ThinPro 7</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>Deploy Files_HP ThinPro 6-64</t>
+          <t>command id</t>
         </is>
       </c>
     </row>
@@ -629,7 +585,302 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet3">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="18.77734375"/>
+    <col customWidth="1" max="3" min="3" style="1" width="9.109375"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="8.33203125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="10.88671875"/>
+    <col customWidth="1" max="234" min="6" style="1" width="9.109375"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>15.83.248.208</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7C:D3:0A:05:01:97</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>15.83.250.20</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>48:0F:CF:BC:DD:3C</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B15:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="3" min="3" style="1" width="9.44140625"/>
+    <col customWidth="1" max="4" min="4" style="1" width="9"/>
+    <col customWidth="1" max="256" min="5" style="1" width="9.109375"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>15.83.250.205</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>48:0F:CF:BB:7C:65</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>15.83.250.210</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>48:0F:CF:BB:7F:65</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet6">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="2" min="1" style="1" width="27.88671875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="22.44140625"/>
+    <col customWidth="1" max="4" min="4" style="1" width="27.33203125"/>
+    <col customWidth="1" max="256" min="5" style="1" width="9.109375"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>WES10IoT-64</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>WES7E</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>WES7P-64</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>HP ThinPro 7</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>CaptureFiles_WES10IoT-64</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>CaptureFiles_WES7E</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>CaptureFiles_WES7P-64</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>CaptureFiles_HP ThinPro 7</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="2">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Command_WES10IoT-64</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Command_WES7E</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Command_WES7P-64</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Command_HP ThinPro 7</t>
+        </is>
+      </c>
+    </row>
+    <row customFormat="1" r="4" s="2">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Files_WES10IoT-64</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Files_WES7E</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Files_WES7P-64</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Deploy Files_HP ThinPro 7</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet7">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -643,7 +894,7 @@
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="9.109375"/>
     <col customWidth="1" max="2" min="2" style="1" width="14.109375"/>
-    <col customWidth="1" max="3" min="3" style="1" width="14.21875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="14.33203125"/>
     <col customWidth="1" max="4" min="4" style="1" width="9.44140625"/>
     <col customWidth="1" max="5" min="5" style="1" width="11.5546875"/>
     <col customWidth="1" max="8" min="6" style="1" width="9.109375"/>

</xml_diff>

<commit_message>
1.modify report email text display 2.modify qtp util, exit qtp after running scripts
</commit_message>
<xml_diff>
--- a/Configuration/test_data.xlsx
+++ b/Configuration/test_data.xlsx
@@ -1,118 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chencar\PycharmProjects\Automation-Framework\Configuration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C1E94-B9D2-4A08-81A9-4856C6196D6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="1" r:id="rId1"/>
-    <sheet name="UUT_HP ThinPro 7" sheetId="2" r:id="rId2"/>
-    <sheet name="UUT_WES7P-64" sheetId="3" r:id="rId3"/>
-    <sheet name="UUT_Win10IoT-64" sheetId="4" r:id="rId4"/>
-    <sheet name="UUT_WES7E" sheetId="5" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UUT_HP ThinPro 7" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UUT_WES7P-64" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UUT_Win10IoT-64" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UUT_WES7E" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Local Path</t>
-  </si>
-  <si>
-    <t>Remote Path</t>
-  </si>
-  <si>
-    <t>Windows_task_2</t>
-  </si>
-  <si>
-    <t>c:/inetpub/ftproot/jenkins/windows/task_2</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Mac</t>
-  </si>
-  <si>
-    <t>capture id</t>
-  </si>
-  <si>
-    <t>deploy id</t>
-  </si>
-  <si>
-    <t>command id</t>
-  </si>
-  <si>
-    <t>15.83.250.20</t>
-  </si>
-  <si>
-    <t>48:0F:CF:BC:DD:3C</t>
-  </si>
-  <si>
-    <t>15.83.248.208</t>
-  </si>
-  <si>
-    <t>7C:D3:0A:05:01:97</t>
-  </si>
-  <si>
-    <r>
-      <t>c:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Mic Shell Dlg"/>
-      </rPr>
-      <t>temp</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
+      <name val="Mic Shell Dlg"/>
       <sz val="10"/>
-      <name val="Mic Shell Dlg"/>
     </font>
     <font>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="DengXian"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -139,26 +66,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -482,254 +400,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:IW2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet5">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="1" customWidth="1"/>
-    <col min="4" max="257" width="9.109375" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="31.88671875"/>
+    <col customWidth="1" max="2" min="2" style="1" width="43.88671875"/>
+    <col customWidth="1" max="3" min="3" style="1" width="21.88671875"/>
+    <col customWidth="1" max="257" min="4" style="1" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Project Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Local Path</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Remote Path</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.8">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
+    <row customHeight="1" ht="13.8" r="2" s="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Windows_task_2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>c:/inetpub/ftproot/jenkins/windows/task_2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>c:/temp</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:IV2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" style="1" customWidth="1"/>
-    <col min="6" max="256" width="9.109375" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="4" min="3" style="1" width="9.109375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="20.5546875"/>
+    <col customWidth="1" max="256" min="6" style="1" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1"/>
+    <row customFormat="1" r="2" s="2"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:IV1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet2">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="256" width="9.109375" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="4" min="3" style="1" width="9.109375"/>
+    <col customWidth="1" max="5" min="5" style="1" width="14"/>
+    <col customWidth="1" max="256" min="6" style="1" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:HZ3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet3">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="234" width="9.109375" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="18.6640625"/>
+    <col customWidth="1" max="3" min="3" style="1" width="9.109375"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="8.33203125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="1" width="10.88671875"/>
+    <col customWidth="1" max="234" min="6" style="1" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>15.83.250.20</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>48:0F:CF:BC:DD:3C</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>15.83.248.208</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7C:D3:0A:05:01:97</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:IV2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="256" width="9.109375" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="12.6640625"/>
+    <col customWidth="1" max="2" min="2" style="1" width="16.33203125"/>
+    <col customWidth="1" max="3" min="3" style="1" width="9.44140625"/>
+    <col customWidth="1" max="4" min="4" style="1" width="9"/>
+    <col customWidth="1" max="256" min="5" style="1" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
+    <row customHeight="1" ht="12.75" r="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mac</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>capture id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>deploy id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>command id</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1"/>
+    <row customFormat="1" r="2" s="2"/>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test_data.xlsx and test_plan2.xlsx
</commit_message>
<xml_diff>
--- a/Configuration/test_data.xlsx
+++ b/Configuration/test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chencar\PycharmProjects\Automation-Framework\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\Automation-Framework\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE740E0B-72A9-48B4-8744-5433AA5340A8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3E3D8C-0960-42BA-95F6-457783E26269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Project Name</t>
   </si>
@@ -64,6 +64,9 @@
   <si>
     <t>Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cycle</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,7 +468,7 @@
   <dimension ref="A1:IW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -476,7 +479,7 @@
     <col min="4" max="257" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +492,11 @@
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="13.8" customHeight="1">
+    <row r="2" spans="1:5" ht="13.8" customHeight="1">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -499,6 +505,9 @@
       </c>
       <c r="C2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -557,7 +566,7 @@
   <dimension ref="A1:IS1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1048576"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>

</xml_diff>